<commit_message>
VS hinzugefügt und an weiteren Profilen gearbeitet
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-t-cabs-communication-alarm.xlsx
+++ b/output/StructureDefinition-t-cabs-communication-alarm.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-03-19T16:19:18+01:00</t>
+    <t>2025-03-25T16:42:03+01:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -643,7 +643,8 @@
   <si>
     <t>&lt;valueCodeableConcept xmlns="http://hl7.org/fhir"&gt;
   &lt;coding&gt;
-    &lt;code value="alert"/&gt;
+    &lt;system value="urn:iso:std:iso:11073:10101"/&gt;
+    &lt;code value="198132"/&gt;
   &lt;/coding&gt;
 &lt;/valueCodeableConcept&gt;</t>
   </si>
@@ -750,7 +751,7 @@
     <t>Resources that pertain to this communication</t>
   </si>
   <si>
-    <t>Der gemessene Wert des Parameters, der die Grenze überschritten hat ((Observation.device auf Messung(DeviceMetric))).</t>
+    <t>Der gemessene Wert des Parameters, der die Alarmgrenze überschritten hat ((Observation.device auf Messung(DeviceMetric))).</t>
   </si>
   <si>
     <t>Don't use Communication.about element when a more specific element exists, such as basedOn or reasonReference.</t>
@@ -3130,7 +3131,7 @@
         <v>85</v>
       </c>
       <c r="H17" t="s" s="2">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="I17" t="s" s="2">
         <v>86</v>
@@ -3463,7 +3464,7 @@
         <v>85</v>
       </c>
       <c r="H20" t="s" s="2">
-        <v>20</v>
+        <v>86</v>
       </c>
       <c r="I20" t="s" s="2">
         <v>20</v>
@@ -3899,7 +3900,7 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>85</v>

</xml_diff>